<commit_message>
commit del 6 de junio
</commit_message>
<xml_diff>
--- a/fe2022 modelado/modeladoprestashop.xlsx
+++ b/fe2022 modelado/modeladoprestashop.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\fe\fe2022 modelado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4512B72E-97EA-4688-931C-379B08017FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AD5866-85F9-4A43-9B3B-E1FF573C45B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -226,7 +226,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +252,14 @@
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -389,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -416,6 +424,8 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,9 +444,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -474,9 +484,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -509,26 +519,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -561,26 +554,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -757,7 +733,7 @@
   <dimension ref="A1:Q60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,10 +1074,10 @@
       </c>
     </row>
     <row r="18" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D18" s="10">
+      <c r="D18" s="26">
         <v>90</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="27">
         <v>36</v>
       </c>
       <c r="F18" s="10" t="s">
@@ -1116,10 +1092,10 @@
       </c>
     </row>
     <row r="19" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D19" s="10">
+      <c r="D19" s="26">
         <v>91</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="27">
         <v>36</v>
       </c>
       <c r="F19" s="10" t="s">
@@ -1134,10 +1110,10 @@
       </c>
     </row>
     <row r="20" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D20" s="10">
+      <c r="D20" s="26">
         <v>92</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="27">
         <v>36</v>
       </c>
       <c r="F20" s="10" t="s">
@@ -1155,10 +1131,10 @@
       </c>
     </row>
     <row r="21" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D21" s="10">
+      <c r="D21" s="26">
         <v>93</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="27">
         <v>36</v>
       </c>
       <c r="F21" s="10" t="s">

</xml_diff>